<commit_message>
Animated title, fixed autoresize, added interest filter.
</commit_message>
<xml_diff>
--- a/parser/data.xlsx
+++ b/parser/data.xlsx
@@ -5,13 +5,15 @@
   <sheets>
     <sheet state="visible" name="Personas" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Personas!$A$1:$F$38</definedName>
+  </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="85">
   <si>
     <t>Persona</t>
   </si>
@@ -91,7 +93,7 @@
     <t>NB</t>
   </si>
   <si>
-    <t>F1, Voley</t>
+    <t>Fórmula 1, Volley</t>
   </si>
   <si>
     <t>Español, Inglés, Frances</t>
@@ -244,6 +246,9 @@
     <t>Camila Cauzzo</t>
   </si>
   <si>
+    <t>Tenis, fútbol</t>
+  </si>
+  <si>
     <t>Juan Castore Bergioli</t>
   </si>
   <si>
@@ -260,9 +265,6 @@
   </si>
   <si>
     <t>Jazz, PostPunk</t>
-  </si>
-  <si>
-    <t>Fúbtbol</t>
   </si>
   <si>
     <t>Jaime Amigo</t>
@@ -330,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -345,6 +347,9 @@
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -599,7 +604,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2">
+    <row r="2" hidden="1">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -619,7 +624,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" hidden="1">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -639,7 +644,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" hidden="1">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -669,7 +674,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6">
+    <row r="6" hidden="1">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -693,13 +698,13 @@
       <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" hidden="1">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
@@ -719,7 +724,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" hidden="1">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
@@ -743,13 +748,13 @@
       <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" hidden="1">
       <c r="A11" s="3" t="s">
         <v>33</v>
       </c>
@@ -773,13 +778,13 @@
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" hidden="1">
       <c r="A13" s="3" t="s">
         <v>36</v>
       </c>
@@ -799,7 +804,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" hidden="1">
       <c r="A14" s="3" t="s">
         <v>39</v>
       </c>
@@ -823,23 +828,23 @@
       <c r="A15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" hidden="1">
       <c r="A17" s="3" t="s">
         <v>44</v>
       </c>
@@ -859,7 +864,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" hidden="1">
       <c r="A18" s="3" t="s">
         <v>47</v>
       </c>
@@ -879,7 +884,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" hidden="1">
       <c r="A19" s="3" t="s">
         <v>51</v>
       </c>
@@ -899,7 +904,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" hidden="1">
       <c r="A20" s="3" t="s">
         <v>54</v>
       </c>
@@ -923,33 +928,33 @@
       <c r="A21" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-    </row>
-    <row r="24">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" hidden="1">
       <c r="A24" s="3" t="s">
         <v>60</v>
       </c>
@@ -969,7 +974,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" hidden="1">
       <c r="A25" s="3" t="s">
         <v>61</v>
       </c>
@@ -989,7 +994,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" hidden="1">
       <c r="A26" s="3" t="s">
         <v>65</v>
       </c>
@@ -1009,7 +1014,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="1">
       <c r="A27" s="3" t="s">
         <v>68</v>
       </c>
@@ -1033,23 +1038,23 @@
       <c r="A28" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-    </row>
-    <row r="30">
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" hidden="1">
       <c r="A30" s="3" t="s">
         <v>73</v>
       </c>
@@ -1069,7 +1074,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" hidden="1">
       <c r="A31" s="3" t="s">
         <v>75</v>
       </c>
@@ -1089,59 +1094,69 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="5" t="s">
+    <row r="32" hidden="1">
+      <c r="A32" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
+      <c r="B32" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
+        <v>78</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
+        <v>79</v>
+      </c>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
+        <v>80</v>
+      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-    </row>
-    <row r="37">
+        <v>81</v>
+      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" hidden="1">
       <c r="A37" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B37" s="4">
         <v>52.0</v>
@@ -1150,10 +1165,10 @@
         <v>12</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>64</v>
@@ -1163,21 +1178,26 @@
       <c r="A38" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
     </row>
     <row r="39">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
     </row>
   </sheetData>
+  <autoFilter ref="$A$1:$F$38">
+    <filterColumn colId="1">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added network auto stabilization zoom.
</commit_message>
<xml_diff>
--- a/parser/data.xlsx
+++ b/parser/data.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Personas" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Variable Types" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Personas!$A$1:$F$38</definedName>
@@ -13,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="99">
   <si>
     <t>Persona</t>
   </si>
@@ -24,7 +25,7 @@
     <t>Género</t>
   </si>
   <si>
-    <t>Género Musical Preferido</t>
+    <t>Género/s Musical/es Preferido/s</t>
   </si>
   <si>
     <t>Deporte/s que mires</t>
@@ -69,7 +70,7 @@
     <t>Curling</t>
   </si>
   <si>
-    <t>Frances, Inglés, Español, Portugues</t>
+    <t>Frances, Inglés, Español, Portugués</t>
   </si>
   <si>
     <t>Tomas Ward</t>
@@ -114,6 +115,15 @@
     <t>Camilo Suárez Canónico</t>
   </si>
   <si>
+    <t>Masculino</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Español, Ingles, Frances</t>
+  </si>
+  <si>
     <t>Franco Setti</t>
   </si>
   <si>
@@ -147,6 +157,12 @@
     <t>Estanislao Rios Zgaib</t>
   </si>
   <si>
+    <t>Tenis</t>
+  </si>
+  <si>
+    <t>Español, Ingles, Italiano</t>
+  </si>
+  <si>
     <t>Federico Peitti</t>
   </si>
   <si>
@@ -174,27 +190,42 @@
     <t>Fútbol, Básquet</t>
   </si>
   <si>
+    <t>Manuel Matías Milde</t>
+  </si>
+  <si>
+    <t>Rock, Jazz</t>
+  </si>
+  <si>
+    <t>Inglés, Español, Portugués</t>
+  </si>
+  <si>
+    <t>Serena Marelli</t>
+  </si>
+  <si>
+    <t>Femenino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rock </t>
+  </si>
+  <si>
+    <t>Futbol</t>
+  </si>
+  <si>
+    <t>Español e inglés</t>
+  </si>
+  <si>
+    <t>Josefina Jahde</t>
+  </si>
+  <si>
+    <t>Iara Guglielmetti</t>
+  </si>
+  <si>
+    <t>Urbano latino</t>
+  </si>
+  <si>
     <t>Español, Ingles</t>
   </si>
   <si>
-    <t>Manuel Matías Milde</t>
-  </si>
-  <si>
-    <t>Rock, Jazz</t>
-  </si>
-  <si>
-    <t>Ingles, Español, Portugués</t>
-  </si>
-  <si>
-    <t>Serena Marelli</t>
-  </si>
-  <si>
-    <t>Josefina Jahde</t>
-  </si>
-  <si>
-    <t>Iara Guglielmetti</t>
-  </si>
-  <si>
     <t>Ezequiel Grinblat</t>
   </si>
   <si>
@@ -268,13 +299,25 @@
   </si>
   <si>
     <t>Jaime Amigo</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Categorico</t>
+  </si>
+  <si>
+    <t>Cuantitativo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -299,8 +342,14 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14.0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,6 +374,18 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF38761D"/>
+        <bgColor rgb="FF38761D"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -332,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -355,6 +416,15 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -364,6 +434,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -574,7 +648,7 @@
     <col customWidth="1" min="1" max="1" width="39.38"/>
     <col customWidth="1" min="2" max="2" width="24.75"/>
     <col customWidth="1" min="3" max="3" width="31.88"/>
-    <col customWidth="1" min="4" max="4" width="39.88"/>
+    <col customWidth="1" min="4" max="4" width="42.13"/>
     <col customWidth="1" min="5" max="5" width="75.25"/>
     <col customWidth="1" min="6" max="6" width="66.38"/>
     <col customWidth="1" min="7" max="7" width="26.0"/>
@@ -744,19 +818,29 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="5" t="s">
+    <row r="10" hidden="1">
+      <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="B10" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="11" hidden="1">
       <c r="A11" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B11" s="4">
         <v>19.0</v>
@@ -768,7 +852,7 @@
         <v>13</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>10</v>
@@ -776,7 +860,7 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -786,7 +870,7 @@
     </row>
     <row r="13" hidden="1">
       <c r="A13" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B13" s="4">
         <v>21.0</v>
@@ -795,10 +879,10 @@
         <v>12</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>10</v>
@@ -806,7 +890,7 @@
     </row>
     <row r="14" hidden="1">
       <c r="A14" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B14" s="4">
         <v>19.0</v>
@@ -818,15 +902,15 @@
         <v>21</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -834,19 +918,29 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16">
-      <c r="A16" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+    <row r="16" hidden="1">
+      <c r="A16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="4">
+        <v>19.0</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="17" hidden="1">
       <c r="A17" s="3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B17" s="4">
         <v>20.0</v>
@@ -855,18 +949,18 @@
         <v>12</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" hidden="1">
       <c r="A18" s="3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B18" s="4">
         <v>20.0</v>
@@ -875,18 +969,18 @@
         <v>7</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" hidden="1">
       <c r="A19" s="3" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B19" s="4">
         <v>19.0</v>
@@ -898,15 +992,15 @@
         <v>13</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" hidden="1">
       <c r="A20" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B20" s="4">
         <v>21.0</v>
@@ -915,48 +1009,67 @@
         <v>12</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" hidden="1">
+      <c r="A21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
       <c r="F22" s="7"/>
     </row>
-    <row r="23">
-      <c r="A23" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+    <row r="23" hidden="1">
+      <c r="A23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="24" hidden="1">
       <c r="A24" s="3" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B24" s="4">
         <v>21.0</v>
@@ -965,7 +1078,7 @@
         <v>12</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>14</v>
@@ -976,7 +1089,7 @@
     </row>
     <row r="25" hidden="1">
       <c r="A25" s="3" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B25" s="4">
         <v>21.0</v>
@@ -985,18 +1098,18 @@
         <v>7</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" hidden="1">
       <c r="A26" s="3" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B26" s="4">
         <v>20.0</v>
@@ -1008,15 +1121,15 @@
         <v>21</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" hidden="1">
       <c r="A27" s="3" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B27" s="4">
         <v>21.0</v>
@@ -1025,10 +1138,10 @@
         <v>12</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>10</v>
@@ -1036,7 +1149,7 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -1044,19 +1157,29 @@
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
     </row>
-    <row r="29">
-      <c r="A29" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
+    <row r="29" hidden="1">
+      <c r="A29" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="30" hidden="1">
       <c r="A30" s="3" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B30" s="4">
         <v>21.0</v>
@@ -1065,7 +1188,7 @@
         <v>12</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>14</v>
@@ -1076,7 +1199,7 @@
     </row>
     <row r="31" hidden="1">
       <c r="A31" s="3" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B31" s="4">
         <v>26.0</v>
@@ -1085,7 +1208,7 @@
         <v>7</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>14</v>
@@ -1096,7 +1219,7 @@
     </row>
     <row r="32" hidden="1">
       <c r="A32" s="3" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B32" s="4">
         <v>21.0</v>
@@ -1108,15 +1231,15 @@
         <v>13</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1126,7 +1249,7 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -1136,7 +1259,7 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -1146,7 +1269,7 @@
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1156,7 +1279,7 @@
     </row>
     <row r="37" hidden="1">
       <c r="A37" s="3" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="B37" s="4">
         <v>52.0</v>
@@ -1165,18 +1288,18 @@
         <v>12</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -1200,4 +1323,79 @@
   </autoFilter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="83.25"/>
+    <col customWidth="1" min="2" max="2" width="50.13"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>